<commit_message>
added new keyword for print mobile name
</commit_message>
<xml_diff>
--- a/src/test/java/stepDefinations/KeywordsFile.xlsx
+++ b/src/test/java/stepDefinations/KeywordsFile.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1724C42B-B6C4-418A-8F0B-42AA01FE5E82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deborah\eclipse-workspace\cucumberAssignment\src\test\java\stepDefinations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E816A5D-3F54-4774-9EAF-860E12DDA8B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="23088" windowHeight="13224" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="verifyText" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
   <si>
     <t>locator</t>
   </si>
@@ -70,9 +74,6 @@
     <t>VERIFY_TEXT</t>
   </si>
   <si>
-    <t>verify text</t>
-  </si>
-  <si>
     <t>id=autoSuggestTxtBox</t>
   </si>
   <si>
@@ -89,6 +90,15 @@
   </si>
   <si>
     <t>id=productCount</t>
+  </si>
+  <si>
+    <t>print mobile name text</t>
+  </si>
+  <si>
+    <t>verify count</t>
+  </si>
+  <si>
+    <t>Print_Mobile_Name</t>
   </si>
 </sst>
 </file>
@@ -437,7 +447,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -492,24 +502,24 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -520,10 +530,10 @@
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>14</v>
@@ -532,21 +542,34 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" display="naveenanimation20@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>